<commit_message>
fix the exact roacle bug by hand
</commit_message>
<xml_diff>
--- a/Linear/EC_Submission/Rounding/Output_Gap/gap_results.xlsx
+++ b/Linear/EC_Submission/Rounding/Output_Gap/gap_results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="54" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="9" uniqueCount="9">
   <si>
     <t>Row</t>
   </si>
@@ -120,16 +120,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>0.0016174318722073089</v>
+        <v>0.0067016980621690259</v>
       </c>
       <c r="C2" s="0">
-        <v>0.00036689744614104569</v>
+        <v>0.00077876288205658284</v>
       </c>
       <c r="D2" s="0">
-        <v>0.00013077251584592275</v>
+        <v>0.00021324968540836764</v>
       </c>
       <c r="E2" s="0">
-        <v>1.6915657997884637e-05</v>
+        <v>0.00011784362499955847</v>
       </c>
     </row>
     <row r="3">
@@ -154,16 +154,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>0.060238740063556229</v>
+        <v>0.01047592140371556</v>
       </c>
       <c r="C4" s="0">
-        <v>0.0015631340031152519</v>
+        <v>0.0072700179959150901</v>
       </c>
       <c r="D4" s="0">
-        <v>0.00087664935862186155</v>
+        <v>0.0091916369931799302</v>
       </c>
       <c r="E4" s="0">
-        <v>0.00072262108074205855</v>
+        <v>0.00099626526775953295</v>
       </c>
     </row>
     <row r="5">
@@ -171,16 +171,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>0.060549144969664459</v>
+        <v>0.0096352374570252142</v>
       </c>
       <c r="C5" s="0">
-        <v>0.022878485874646248</v>
+        <v>0.018987640380649928</v>
       </c>
       <c r="D5" s="0">
-        <v>0.0034639364758746183</v>
+        <v>0.015372356185406222</v>
       </c>
       <c r="E5" s="0">
-        <v>0.003396300030098498</v>
+        <v>0.0034478576400140959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>